<commit_message>
2 Signed-off-by: zhoujunren <195913@baosight.com>
</commit_message>
<xml_diff>
--- a/类线性关系拟合/updated_excel_file.xlsx
+++ b/类线性关系拟合/updated_excel_file.xlsx
@@ -423,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>6.876562499999999</v>
+        <v>6.8765625</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>6.625763888888898</v>
+        <v>6.6257638888889</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>6.753147208121902</v>
+        <v>6.7531472081219</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>7.665891089109003</v>
+        <v>7.665891089109</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>7.095466101694996</v>
+        <v>7.095466101695</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -542,7 +542,7 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>7.199775280898905</v>
+        <v>7.1997752808989</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -559,7 +559,7 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <v>7.530236966824695</v>
+        <v>7.5302369668247</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -576,7 +576,7 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>7.481935483871005</v>
+        <v>7.481935483871</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -610,7 +610,7 @@
         <v>13</v>
       </c>
       <c r="E13">
-        <v>7.150937500000005</v>
+        <v>7.1509375</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -627,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="E14">
-        <v>7.612439024390298</v>
+        <v>7.6124390243903</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -661,7 +661,7 @@
         <v>16</v>
       </c>
       <c r="E16">
-        <v>7.353076923076998</v>
+        <v>7.353076923077</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -712,7 +712,7 @@
         <v>19</v>
       </c>
       <c r="E19">
-        <v>7.595945945946006</v>
+        <v>7.59594594594601</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -729,7 +729,7 @@
         <v>20</v>
       </c>
       <c r="E20">
-        <v>7.811058201058302</v>
+        <v>7.8110582010583</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -746,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="E21">
-        <v>7.670129870129898</v>
+        <v>7.6701298701299</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -763,7 +763,7 @@
         <v>22</v>
       </c>
       <c r="E22">
-        <v>7.698571428571505</v>
+        <v>7.6985714285715</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -780,7 +780,7 @@
         <v>23</v>
       </c>
       <c r="E23">
-        <v>7.320585585585597</v>
+        <v>7.3205855855856</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -797,7 +797,7 @@
         <v>24</v>
       </c>
       <c r="E24">
-        <v>7.410279329608997</v>
+        <v>7.410279329609</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -814,7 +814,7 @@
         <v>25</v>
       </c>
       <c r="E25">
-        <v>7.492675159235695</v>
+        <v>7.4926751592357</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -831,7 +831,7 @@
         <v>26</v>
       </c>
       <c r="E26">
-        <v>7.271860465116305</v>
+        <v>7.2718604651163</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1018,7 +1018,7 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>6.875707762557099</v>
+        <v>6.8757077625571</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1052,7 +1052,7 @@
         <v>43</v>
       </c>
       <c r="E39">
-        <v>6.650694444444497</v>
+        <v>6.6506944444445</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1069,7 +1069,7 @@
         <v>44</v>
       </c>
       <c r="E40">
-        <v>6.966553672316401</v>
+        <v>6.9665536723164</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1086,7 +1086,7 @@
         <v>45</v>
       </c>
       <c r="E41">
-        <v>7.028435754189999</v>
+        <v>7.02843575419</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1120,7 +1120,7 @@
         <v>47</v>
       </c>
       <c r="E43">
-        <v>6.719117647058901</v>
+        <v>6.7191176470589</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1137,7 +1137,7 @@
         <v>48</v>
       </c>
       <c r="E44">
-        <v>6.637473118279594</v>
+        <v>6.63747311827959</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1154,7 +1154,7 @@
         <v>49</v>
       </c>
       <c r="E45">
-        <v>6.813333333333404</v>
+        <v>6.8133333333334</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1171,7 +1171,7 @@
         <v>50</v>
       </c>
       <c r="E46">
-        <v>6.202514970059902</v>
+        <v>6.2025149700599</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1188,7 +1188,7 @@
         <v>51</v>
       </c>
       <c r="E47">
-        <v>6.737802197802196</v>
+        <v>6.7378021978022</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1222,7 +1222,7 @@
         <v>53</v>
       </c>
       <c r="E49">
-        <v>6.686296296296298</v>
+        <v>6.6862962962963</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1239,7 +1239,7 @@
         <v>54</v>
       </c>
       <c r="E50">
-        <v>6.695751295336798</v>
+        <v>6.6957512953368</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1256,7 +1256,7 @@
         <v>55</v>
       </c>
       <c r="E51">
-        <v>7.136289308176202</v>
+        <v>7.1362893081762</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1273,7 +1273,7 @@
         <v>56</v>
       </c>
       <c r="E52">
-        <v>6.914383561643902</v>
+        <v>6.9143835616439</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1307,7 +1307,7 @@
         <v>58</v>
       </c>
       <c r="E54">
-        <v>7.046158940397397</v>
+        <v>7.0461589403974</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1324,7 +1324,7 @@
         <v>59</v>
       </c>
       <c r="E55">
-        <v>7.042857142857201</v>
+        <v>7.0428571428572</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1341,7 +1341,7 @@
         <v>60</v>
       </c>
       <c r="E56">
-        <v>6.762539682539696</v>
+        <v>6.7625396825397</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1358,7 +1358,7 @@
         <v>61</v>
       </c>
       <c r="E57">
-        <v>7.325317919075196</v>
+        <v>7.3253179190752</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1375,7 +1375,7 @@
         <v>62</v>
       </c>
       <c r="E58">
-        <v>7.646176470588294</v>
+        <v>7.64617647058829</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1409,7 +1409,7 @@
         <v>64</v>
       </c>
       <c r="E60">
-        <v>7.515069444444499</v>
+        <v>7.5150694444445</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1426,7 +1426,7 @@
         <v>65</v>
       </c>
       <c r="E61">
-        <v>7.187560975609799</v>
+        <v>7.1875609756098</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1443,7 +1443,7 @@
         <v>66</v>
       </c>
       <c r="E62">
-        <v>7.358037974683597</v>
+        <v>7.3580379746836</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1460,7 +1460,7 @@
         <v>67</v>
       </c>
       <c r="E63">
-        <v>6.917961165048602</v>
+        <v>6.9179611650486</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1511,7 +1511,7 @@
         <v>70</v>
       </c>
       <c r="E66">
-        <v>6.461666666666702</v>
+        <v>6.4616666666667</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1528,7 +1528,7 @@
         <v>71</v>
       </c>
       <c r="E67">
-        <v>6.502950819672201</v>
+        <v>6.5029508196722</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1545,7 +1545,7 @@
         <v>72</v>
       </c>
       <c r="E68">
-        <v>7.243471502590701</v>
+        <v>7.2434715025907</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1562,7 +1562,7 @@
         <v>73</v>
       </c>
       <c r="E69">
-        <v>6.937209302325599</v>
+        <v>6.9372093023256</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1596,7 +1596,7 @@
         <v>75</v>
       </c>
       <c r="E71">
-        <v>6.610277777777803</v>
+        <v>6.6102777777778</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1613,7 +1613,7 @@
         <v>76</v>
       </c>
       <c r="E72">
-        <v>6.547142857142902</v>
+        <v>6.5471428571429</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1630,7 +1630,7 @@
         <v>77</v>
       </c>
       <c r="E73">
-        <v>6.463214285714301</v>
+        <v>6.4632142857143</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1647,7 +1647,7 @@
         <v>78</v>
       </c>
       <c r="E74">
-        <v>7.714924471299099</v>
+        <v>7.7149244712991</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1664,7 +1664,7 @@
         <v>79</v>
       </c>
       <c r="E75">
-        <v>6.699839572192595</v>
+        <v>6.6998395721926</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1681,7 +1681,7 @@
         <v>80</v>
       </c>
       <c r="E76">
-        <v>6.549047619047698</v>
+        <v>6.5490476190477</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1698,7 +1698,7 @@
         <v>81</v>
       </c>
       <c r="E77">
-        <v>6.138394160583999</v>
+        <v>6.138394160584</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1732,7 +1732,7 @@
         <v>83</v>
       </c>
       <c r="E79">
-        <v>6.651402714932196</v>
+        <v>6.6514027149322</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1749,7 +1749,7 @@
         <v>84</v>
       </c>
       <c r="E80">
-        <v>6.532237762237806</v>
+        <v>6.53223776223781</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1766,7 +1766,7 @@
         <v>85</v>
       </c>
       <c r="E81">
-        <v>6.431629213483198</v>
+        <v>6.4316292134832</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1783,7 +1783,7 @@
         <v>86</v>
       </c>
       <c r="E82">
-        <v>6.787777777777798</v>
+        <v>6.7877777777778</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1800,7 +1800,7 @@
         <v>87</v>
       </c>
       <c r="E83">
-        <v>6.695631067961195</v>
+        <v>6.69563106796119</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1817,7 +1817,7 @@
         <v>88</v>
       </c>
       <c r="E84">
-        <v>6.800312500000004</v>
+        <v>6.8003125</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1834,7 +1834,7 @@
         <v>89</v>
       </c>
       <c r="E85">
-        <v>6.598587570621504</v>
+        <v>6.5985875706215</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1851,7 +1851,7 @@
         <v>90</v>
       </c>
       <c r="E86">
-        <v>6.742176165803201</v>
+        <v>6.7421761658032</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1868,7 +1868,7 @@
         <v>91</v>
       </c>
       <c r="E87">
-        <v>6.788030303030396</v>
+        <v>6.7880303030304</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1885,7 +1885,7 @@
         <v>92</v>
       </c>
       <c r="E88">
-        <v>6.777272727272802</v>
+        <v>6.7772727272728</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1902,7 +1902,7 @@
         <v>93</v>
       </c>
       <c r="E89">
-        <v>6.406860068259398</v>
+        <v>6.4068600682594</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1919,7 +1919,7 @@
         <v>94</v>
       </c>
       <c r="E90">
-        <v>7.160532544378697</v>
+        <v>7.1605325443787</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1936,7 +1936,7 @@
         <v>95</v>
       </c>
       <c r="E91">
-        <v>7.916054421768798</v>
+        <v>7.9160544217688</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1953,7 +1953,7 @@
         <v>96</v>
       </c>
       <c r="E92">
-        <v>6.763734939759097</v>
+        <v>6.7637349397591</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2038,7 +2038,7 @@
         <v>103</v>
       </c>
       <c r="E97">
-        <v>6.668984771573697</v>
+        <v>6.6689847715737</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2055,7 +2055,7 @@
         <v>104</v>
       </c>
       <c r="E98">
-        <v>6.932317880794798</v>
+        <v>6.9323178807948</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2072,7 +2072,7 @@
         <v>105</v>
       </c>
       <c r="E99">
-        <v>7.029905660377402</v>
+        <v>7.0299056603774</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2089,7 +2089,7 @@
         <v>106</v>
       </c>
       <c r="E100">
-        <v>6.607187500000002</v>
+        <v>6.6071875</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2106,7 +2106,7 @@
         <v>107</v>
       </c>
       <c r="E101">
-        <v>6.617386363636399</v>
+        <v>6.6173863636364</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2123,7 +2123,7 @@
         <v>108</v>
       </c>
       <c r="E102">
-        <v>6.655698924731198</v>
+        <v>6.6556989247312</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2140,7 +2140,7 @@
         <v>109</v>
       </c>
       <c r="E103">
-        <v>6.650962343096296</v>
+        <v>6.6509623430963</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2157,7 +2157,7 @@
         <v>110</v>
       </c>
       <c r="E104">
-        <v>6.807086092715295</v>
+        <v>6.80708609271529</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2174,7 +2174,7 @@
         <v>111</v>
       </c>
       <c r="E105">
-        <v>6.476216216216301</v>
+        <v>6.4762162162163</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2191,7 +2191,7 @@
         <v>112</v>
       </c>
       <c r="E106">
-        <v>6.461797235023106</v>
+        <v>6.46179723502311</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2208,7 +2208,7 @@
         <v>113</v>
       </c>
       <c r="E107">
-        <v>6.380331125827901</v>
+        <v>6.3803311258279</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2225,7 +2225,7 @@
         <v>114</v>
       </c>
       <c r="E108">
-        <v>6.509107142857204</v>
+        <v>6.5091071428572</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2276,7 +2276,7 @@
         <v>117</v>
       </c>
       <c r="E111">
-        <v>6.871165644171803</v>
+        <v>6.8711656441718</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2293,7 +2293,7 @@
         <v>118</v>
       </c>
       <c r="E112">
-        <v>6.879512195121997</v>
+        <v>6.879512195122</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2310,7 +2310,7 @@
         <v>119</v>
       </c>
       <c r="E113">
-        <v>6.709216867469898</v>
+        <v>6.7092168674699</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2344,7 +2344,7 @@
         <v>121</v>
       </c>
       <c r="E115">
-        <v>6.995324675324703</v>
+        <v>6.9953246753247</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2361,7 +2361,7 @@
         <v>122</v>
       </c>
       <c r="E116">
-        <v>6.693333333333399</v>
+        <v>6.6933333333334</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2378,7 +2378,7 @@
         <v>123</v>
       </c>
       <c r="E117">
-        <v>6.948333333333402</v>
+        <v>6.9483333333334</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2395,7 +2395,7 @@
         <v>124</v>
       </c>
       <c r="E118">
-        <v>6.778349514563203</v>
+        <v>6.7783495145632</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2412,7 +2412,7 @@
         <v>125</v>
       </c>
       <c r="E119">
-        <v>7.333892215568902</v>
+        <v>7.3338922155689</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2446,7 +2446,7 @@
         <v>127</v>
       </c>
       <c r="E121">
-        <v>7.168333333333401</v>
+        <v>7.1683333333334</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2463,7 +2463,7 @@
         <v>128</v>
       </c>
       <c r="E122">
-        <v>6.618464730290498</v>
+        <v>6.6184647302905</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2480,7 +2480,7 @@
         <v>129</v>
       </c>
       <c r="E123">
-        <v>6.712015503875996</v>
+        <v>6.712015503876</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2497,7 +2497,7 @@
         <v>130</v>
       </c>
       <c r="E124">
-        <v>6.922896174863396</v>
+        <v>6.9228961748634</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2514,7 +2514,7 @@
         <v>131</v>
       </c>
       <c r="E125">
-        <v>8.687000000000005</v>
+        <v>8.686999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2531,7 +2531,7 @@
         <v>132</v>
       </c>
       <c r="E126">
-        <v>6.910829015544103</v>
+        <v>6.9108290155441</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2548,7 +2548,7 @@
         <v>133</v>
       </c>
       <c r="E127">
-        <v>7.403245149911903</v>
+        <v>7.4032451499119</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2565,7 +2565,7 @@
         <v>134</v>
       </c>
       <c r="E128">
-        <v>6.692232415902197</v>
+        <v>6.6922324159022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>